<commit_message>
More Excel data files.
</commit_message>
<xml_diff>
--- a/CivilWars.xlsx
+++ b/CivilWars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18613"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F0E76B5-8905-4427-BBF1-E972DFC05B10}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37804A3A-1436-489D-A86C-729B2830BE86}" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179020"/>
+  <calcPr calcId="171026"/>
 </workbook>
 </file>
 

</xml_diff>